<commit_message>
translating comments in english
</commit_message>
<xml_diff>
--- a/random_data/list_data_table1.xlsx
+++ b/random_data/list_data_table1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/onedrive-univ-pd/pedagogical_projects/pedagogical_extended_prone/random_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/onedrive-univ-pd/pedagogical_extended_prone/random_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68701D2B-390F-CC49-97EC-02118C8AE8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4442A3-66E2-354E-AB25-77B13110888C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{046C0BB0-E403-0846-AC83-4DDD031FA42B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{046C0BB0-E403-0846-AC83-4DDD031FA42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>At least one proning session with catecholamines</t>
   </si>
   <si>
-    <t>fdr</t>
-  </si>
-  <si>
     <t>prévu</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>drvp_bfr_pp</t>
+  </si>
+  <si>
+    <t>risk_factor</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +749,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -761,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -778,12 +778,12 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -795,12 +795,12 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -826,15 +826,15 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -871,12 +871,12 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -885,10 +885,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -902,10 +902,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -919,15 +919,15 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -936,12 +936,12 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -950,12 +950,12 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -964,57 +964,57 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1023,40 +1023,40 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1064,305 +1064,305 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
         <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
         <v>48</v>
       </c>
-      <c r="B35" t="s">
-        <v>49</v>
-      </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated a bunch of files
</commit_message>
<xml_diff>
--- a/random_data/list_data_table1.xlsx
+++ b/random_data/list_data_table1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/onedrive-univ-pd/pedagogical_extended_prone/random_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4442A3-66E2-354E-AB25-77B13110888C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A2788A-A584-3541-837F-5F25186B11CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{046C0BB0-E403-0846-AC83-4DDD031FA42B}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="29280" windowHeight="18880" xr2:uid="{046C0BB0-E403-0846-AC83-4DDD031FA42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>table</t>
   </si>
   <si>
-    <t>Sex, male</t>
-  </si>
-  <si>
     <t>Active smoker</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>risk_factor</t>
+  </si>
+  <si>
+    <t>Sex, feminine</t>
   </si>
 </sst>
 </file>
@@ -395,15 +395,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +718,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +729,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -744,625 +741,625 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
         <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>55</v>
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="E45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="E46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="E48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="E49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E49" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E50" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="E51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>